<commit_message>
Text - Performance chapter, comparing prototype vs final system
</commit_message>
<xml_diff>
--- a/Text/diagrams/PerformanceData.xlsx
+++ b/Text/diagrams/PerformanceData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VUT FIT\9. semestr\SEP\Diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VUT FIT\10. semestr\DIP\Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665A4925-48C1-41EA-991F-E132541E2A02}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{672CF487-883E-4863-82CE-64E196487AE5}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>Count</t>
   </si>
@@ -45,6 +46,12 @@
   </si>
   <si>
     <t>AVG packet size (Bytes)</t>
+  </si>
+  <si>
+    <t>Prototyp</t>
+  </si>
+  <si>
+    <t>Finální systém</t>
   </si>
 </sst>
 </file>
@@ -398,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4576FBAD-09E4-4755-A91C-BDE86BD7E3A1}">
-  <dimension ref="D4:K9"/>
+  <dimension ref="D3:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,6 +420,11 @@
     <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>4</v>
@@ -537,6 +549,137 @@
       <c r="H9">
         <f>E9/G9</f>
         <v>88.379310344827587</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <v>91340</v>
+      </c>
+      <c r="E13">
+        <v>382</v>
+      </c>
+      <c r="F13">
+        <f>D13/E13</f>
+        <v>239.10994764397907</v>
+      </c>
+      <c r="G13">
+        <v>0.5</v>
+      </c>
+      <c r="H13">
+        <f>E13/G13</f>
+        <v>764</v>
+      </c>
+      <c r="J13">
+        <f>AVERAGEA(H13:H17)</f>
+        <v>2242.7333333333331</v>
+      </c>
+      <c r="K13">
+        <f>AVERAGEA(F13:F17)</f>
+        <v>451.47842791727788</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>1955172</v>
+      </c>
+      <c r="E14">
+        <v>1360</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F17" si="1">D14/E14</f>
+        <v>1437.6264705882354</v>
+      </c>
+      <c r="G14">
+        <v>0.5</v>
+      </c>
+      <c r="H14">
+        <f>E14/G14</f>
+        <v>2720</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <v>412254</v>
+      </c>
+      <c r="E15">
+        <v>1879</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>219.40074507716869</v>
+      </c>
+      <c r="G15">
+        <v>0.5</v>
+      </c>
+      <c r="H15">
+        <f>E15/G15</f>
+        <v>3758</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>420869</v>
+      </c>
+      <c r="E16">
+        <v>2263</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>185.97834732655767</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <f>E16/G16</f>
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="1">
+        <v>449234</v>
+      </c>
+      <c r="E17">
+        <v>2563</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>175.2766289504487</v>
+      </c>
+      <c r="G17">
+        <v>1.5</v>
+      </c>
+      <c r="H17">
+        <f>E17/G17</f>
+        <v>1708.6666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>